<commit_message>
Template: Freeze first row + first column
Test that Stata excel export keeps the frozen view settings on the
sheets. It works excellent!
</commit_message>
<xml_diff>
--- a/sdgindex.xlsx
+++ b/sdgindex.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Finn Woelm\Projects\stata-excel-template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C6B9D0-E910-491C-92AA-CC4ADA4050E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB2072B-F8E2-409C-8D0F-A5FF66218538}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="945" yWindow="1410" windowWidth="23040" windowHeight="11835"/>
+    <workbookView xWindow="945" yWindow="1410" windowWidth="23040" windowHeight="11835" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Results" sheetId="8" r:id="rId1"/>
@@ -1808,7 +1808,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CAFD747-961D-4958-B282-966AFB409A3E}">
   <dimension ref="A1:N75"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5159,7 +5164,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3AF4C6E-3E65-4E26-AFB9-A800448A3220}">
   <dimension ref="A1:N75"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8539,8 +8549,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81D59EDA-29EF-4B54-BF6D-02E731E6D405}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="true" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Bold & slant header row
Use Stata's excelput command to apply "normal" formatting to the Excel 
file. In this case, we're boldening and slanting by 45 degrees the 
header row.
</commit_message>
<xml_diff>
--- a/sdgindex.xlsx
+++ b/sdgindex.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -368,6 +368,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+    </font>
+    <font>
+      <b/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -377,7 +383,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -388,12 +394,14 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true"/>
@@ -410,6 +418,12 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="true">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="true">
+      <alignment textRotation="45"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1818,7 +1832,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CAFD747-961D-4958-B282-966AFB409A3E}">
-  <dimension ref="A1:N75"/>
+  <dimension ref="A1:ZZ75"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -1835,48 +1849,736 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="10" t="s">
         <v>96</v>
       </c>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10"/>
+      <c r="Z1" s="10"/>
+      <c r="AA1" s="10"/>
+      <c r="AB1" s="10"/>
+      <c r="AC1" s="10"/>
+      <c r="AD1" s="10"/>
+      <c r="AE1" s="10"/>
+      <c r="AF1" s="10"/>
+      <c r="AG1" s="10"/>
+      <c r="AH1" s="10"/>
+      <c r="AI1" s="10"/>
+      <c r="AJ1" s="10"/>
+      <c r="AK1" s="10"/>
+      <c r="AL1" s="10"/>
+      <c r="AM1" s="10"/>
+      <c r="AN1" s="10"/>
+      <c r="AO1" s="10"/>
+      <c r="AP1" s="10"/>
+      <c r="AQ1" s="10"/>
+      <c r="AR1" s="10"/>
+      <c r="AS1" s="10"/>
+      <c r="AT1" s="10"/>
+      <c r="AU1" s="10"/>
+      <c r="AV1" s="10"/>
+      <c r="AW1" s="10"/>
+      <c r="AX1" s="10"/>
+      <c r="AY1" s="10"/>
+      <c r="AZ1" s="10"/>
+      <c r="BA1" s="10"/>
+      <c r="BB1" s="10"/>
+      <c r="BC1" s="10"/>
+      <c r="BD1" s="10"/>
+      <c r="BE1" s="10"/>
+      <c r="BF1" s="10"/>
+      <c r="BG1" s="10"/>
+      <c r="BH1" s="10"/>
+      <c r="BI1" s="10"/>
+      <c r="BJ1" s="10"/>
+      <c r="BK1" s="10"/>
+      <c r="BL1" s="10"/>
+      <c r="BM1" s="10"/>
+      <c r="BN1" s="10"/>
+      <c r="BO1" s="10"/>
+      <c r="BP1" s="10"/>
+      <c r="BQ1" s="10"/>
+      <c r="BR1" s="10"/>
+      <c r="BS1" s="10"/>
+      <c r="BT1" s="10"/>
+      <c r="BU1" s="10"/>
+      <c r="BV1" s="10"/>
+      <c r="BW1" s="10"/>
+      <c r="BX1" s="10"/>
+      <c r="BY1" s="10"/>
+      <c r="BZ1" s="10"/>
+      <c r="CA1" s="10"/>
+      <c r="CB1" s="10"/>
+      <c r="CC1" s="10"/>
+      <c r="CD1" s="10"/>
+      <c r="CE1" s="10"/>
+      <c r="CF1" s="10"/>
+      <c r="CG1" s="10"/>
+      <c r="CH1" s="10"/>
+      <c r="CI1" s="10"/>
+      <c r="CJ1" s="10"/>
+      <c r="CK1" s="10"/>
+      <c r="CL1" s="10"/>
+      <c r="CM1" s="10"/>
+      <c r="CN1" s="10"/>
+      <c r="CO1" s="10"/>
+      <c r="CP1" s="10"/>
+      <c r="CQ1" s="10"/>
+      <c r="CR1" s="10"/>
+      <c r="CS1" s="10"/>
+      <c r="CT1" s="10"/>
+      <c r="CU1" s="10"/>
+      <c r="CV1" s="10"/>
+      <c r="CW1" s="10"/>
+      <c r="CX1" s="10"/>
+      <c r="CY1" s="10"/>
+      <c r="CZ1" s="10"/>
+      <c r="DA1" s="10"/>
+      <c r="DB1" s="10"/>
+      <c r="DC1" s="10"/>
+      <c r="DD1" s="10"/>
+      <c r="DE1" s="10"/>
+      <c r="DF1" s="10"/>
+      <c r="DG1" s="10"/>
+      <c r="DH1" s="10"/>
+      <c r="DI1" s="10"/>
+      <c r="DJ1" s="10"/>
+      <c r="DK1" s="10"/>
+      <c r="DL1" s="10"/>
+      <c r="DM1" s="10"/>
+      <c r="DN1" s="10"/>
+      <c r="DO1" s="10"/>
+      <c r="DP1" s="10"/>
+      <c r="DQ1" s="10"/>
+      <c r="DR1" s="10"/>
+      <c r="DS1" s="10"/>
+      <c r="DT1" s="10"/>
+      <c r="DU1" s="10"/>
+      <c r="DV1" s="10"/>
+      <c r="DW1" s="10"/>
+      <c r="DX1" s="10"/>
+      <c r="DY1" s="10"/>
+      <c r="DZ1" s="10"/>
+      <c r="EA1" s="10"/>
+      <c r="EB1" s="10"/>
+      <c r="EC1" s="10"/>
+      <c r="ED1" s="10"/>
+      <c r="EE1" s="10"/>
+      <c r="EF1" s="10"/>
+      <c r="EG1" s="10"/>
+      <c r="EH1" s="10"/>
+      <c r="EI1" s="10"/>
+      <c r="EJ1" s="10"/>
+      <c r="EK1" s="10"/>
+      <c r="EL1" s="10"/>
+      <c r="EM1" s="10"/>
+      <c r="EN1" s="10"/>
+      <c r="EO1" s="10"/>
+      <c r="EP1" s="10"/>
+      <c r="EQ1" s="10"/>
+      <c r="ER1" s="10"/>
+      <c r="ES1" s="10"/>
+      <c r="ET1" s="10"/>
+      <c r="EU1" s="10"/>
+      <c r="EV1" s="10"/>
+      <c r="EW1" s="10"/>
+      <c r="EX1" s="10"/>
+      <c r="EY1" s="10"/>
+      <c r="EZ1" s="10"/>
+      <c r="FA1" s="10"/>
+      <c r="FB1" s="10"/>
+      <c r="FC1" s="10"/>
+      <c r="FD1" s="10"/>
+      <c r="FE1" s="10"/>
+      <c r="FF1" s="10"/>
+      <c r="FG1" s="10"/>
+      <c r="FH1" s="10"/>
+      <c r="FI1" s="10"/>
+      <c r="FJ1" s="10"/>
+      <c r="FK1" s="10"/>
+      <c r="FL1" s="10"/>
+      <c r="FM1" s="10"/>
+      <c r="FN1" s="10"/>
+      <c r="FO1" s="10"/>
+      <c r="FP1" s="10"/>
+      <c r="FQ1" s="10"/>
+      <c r="FR1" s="10"/>
+      <c r="FS1" s="10"/>
+      <c r="FT1" s="10"/>
+      <c r="FU1" s="10"/>
+      <c r="FV1" s="10"/>
+      <c r="FW1" s="10"/>
+      <c r="FX1" s="10"/>
+      <c r="FY1" s="10"/>
+      <c r="FZ1" s="10"/>
+      <c r="GA1" s="10"/>
+      <c r="GB1" s="10"/>
+      <c r="GC1" s="10"/>
+      <c r="GD1" s="10"/>
+      <c r="GE1" s="10"/>
+      <c r="GF1" s="10"/>
+      <c r="GG1" s="10"/>
+      <c r="GH1" s="10"/>
+      <c r="GI1" s="10"/>
+      <c r="GJ1" s="10"/>
+      <c r="GK1" s="10"/>
+      <c r="GL1" s="10"/>
+      <c r="GM1" s="10"/>
+      <c r="GN1" s="10"/>
+      <c r="GO1" s="10"/>
+      <c r="GP1" s="10"/>
+      <c r="GQ1" s="10"/>
+      <c r="GR1" s="10"/>
+      <c r="GS1" s="10"/>
+      <c r="GT1" s="10"/>
+      <c r="GU1" s="10"/>
+      <c r="GV1" s="10"/>
+      <c r="GW1" s="10"/>
+      <c r="GX1" s="10"/>
+      <c r="GY1" s="10"/>
+      <c r="GZ1" s="10"/>
+      <c r="HA1" s="10"/>
+      <c r="HB1" s="10"/>
+      <c r="HC1" s="10"/>
+      <c r="HD1" s="10"/>
+      <c r="HE1" s="10"/>
+      <c r="HF1" s="10"/>
+      <c r="HG1" s="10"/>
+      <c r="HH1" s="10"/>
+      <c r="HI1" s="10"/>
+      <c r="HJ1" s="10"/>
+      <c r="HK1" s="10"/>
+      <c r="HL1" s="10"/>
+      <c r="HM1" s="10"/>
+      <c r="HN1" s="10"/>
+      <c r="HO1" s="10"/>
+      <c r="HP1" s="10"/>
+      <c r="HQ1" s="10"/>
+      <c r="HR1" s="10"/>
+      <c r="HS1" s="10"/>
+      <c r="HT1" s="10"/>
+      <c r="HU1" s="10"/>
+      <c r="HV1" s="10"/>
+      <c r="HW1" s="10"/>
+      <c r="HX1" s="10"/>
+      <c r="HY1" s="10"/>
+      <c r="HZ1" s="10"/>
+      <c r="IA1" s="10"/>
+      <c r="IB1" s="10"/>
+      <c r="IC1" s="10"/>
+      <c r="ID1" s="10"/>
+      <c r="IE1" s="10"/>
+      <c r="IF1" s="10"/>
+      <c r="IG1" s="10"/>
+      <c r="IH1" s="10"/>
+      <c r="II1" s="10"/>
+      <c r="IJ1" s="10"/>
+      <c r="IK1" s="10"/>
+      <c r="IL1" s="10"/>
+      <c r="IM1" s="10"/>
+      <c r="IN1" s="10"/>
+      <c r="IO1" s="10"/>
+      <c r="IP1" s="10"/>
+      <c r="IQ1" s="10"/>
+      <c r="IR1" s="10"/>
+      <c r="IS1" s="10"/>
+      <c r="IT1" s="10"/>
+      <c r="IU1" s="10"/>
+      <c r="IV1" s="10"/>
+      <c r="IW1" s="10"/>
+      <c r="IX1" s="10"/>
+      <c r="IY1" s="10"/>
+      <c r="IZ1" s="10"/>
+      <c r="JA1" s="10"/>
+      <c r="JB1" s="10"/>
+      <c r="JC1" s="10"/>
+      <c r="JD1" s="10"/>
+      <c r="JE1" s="10"/>
+      <c r="JF1" s="10"/>
+      <c r="JG1" s="10"/>
+      <c r="JH1" s="10"/>
+      <c r="JI1" s="10"/>
+      <c r="JJ1" s="10"/>
+      <c r="JK1" s="10"/>
+      <c r="JL1" s="10"/>
+      <c r="JM1" s="10"/>
+      <c r="JN1" s="10"/>
+      <c r="JO1" s="10"/>
+      <c r="JP1" s="10"/>
+      <c r="JQ1" s="10"/>
+      <c r="JR1" s="10"/>
+      <c r="JS1" s="10"/>
+      <c r="JT1" s="10"/>
+      <c r="JU1" s="10"/>
+      <c r="JV1" s="10"/>
+      <c r="JW1" s="10"/>
+      <c r="JX1" s="10"/>
+      <c r="JY1" s="10"/>
+      <c r="JZ1" s="10"/>
+      <c r="KA1" s="10"/>
+      <c r="KB1" s="10"/>
+      <c r="KC1" s="10"/>
+      <c r="KD1" s="10"/>
+      <c r="KE1" s="10"/>
+      <c r="KF1" s="10"/>
+      <c r="KG1" s="10"/>
+      <c r="KH1" s="10"/>
+      <c r="KI1" s="10"/>
+      <c r="KJ1" s="10"/>
+      <c r="KK1" s="10"/>
+      <c r="KL1" s="10"/>
+      <c r="KM1" s="10"/>
+      <c r="KN1" s="10"/>
+      <c r="KO1" s="10"/>
+      <c r="KP1" s="10"/>
+      <c r="KQ1" s="10"/>
+      <c r="KR1" s="10"/>
+      <c r="KS1" s="10"/>
+      <c r="KT1" s="10"/>
+      <c r="KU1" s="10"/>
+      <c r="KV1" s="10"/>
+      <c r="KW1" s="10"/>
+      <c r="KX1" s="10"/>
+      <c r="KY1" s="10"/>
+      <c r="KZ1" s="10"/>
+      <c r="LA1" s="10"/>
+      <c r="LB1" s="10"/>
+      <c r="LC1" s="10"/>
+      <c r="LD1" s="10"/>
+      <c r="LE1" s="10"/>
+      <c r="LF1" s="10"/>
+      <c r="LG1" s="10"/>
+      <c r="LH1" s="10"/>
+      <c r="LI1" s="10"/>
+      <c r="LJ1" s="10"/>
+      <c r="LK1" s="10"/>
+      <c r="LL1" s="10"/>
+      <c r="LM1" s="10"/>
+      <c r="LN1" s="10"/>
+      <c r="LO1" s="10"/>
+      <c r="LP1" s="10"/>
+      <c r="LQ1" s="10"/>
+      <c r="LR1" s="10"/>
+      <c r="LS1" s="10"/>
+      <c r="LT1" s="10"/>
+      <c r="LU1" s="10"/>
+      <c r="LV1" s="10"/>
+      <c r="LW1" s="10"/>
+      <c r="LX1" s="10"/>
+      <c r="LY1" s="10"/>
+      <c r="LZ1" s="10"/>
+      <c r="MA1" s="10"/>
+      <c r="MB1" s="10"/>
+      <c r="MC1" s="10"/>
+      <c r="MD1" s="10"/>
+      <c r="ME1" s="10"/>
+      <c r="MF1" s="10"/>
+      <c r="MG1" s="10"/>
+      <c r="MH1" s="10"/>
+      <c r="MI1" s="10"/>
+      <c r="MJ1" s="10"/>
+      <c r="MK1" s="10"/>
+      <c r="ML1" s="10"/>
+      <c r="MM1" s="10"/>
+      <c r="MN1" s="10"/>
+      <c r="MO1" s="10"/>
+      <c r="MP1" s="10"/>
+      <c r="MQ1" s="10"/>
+      <c r="MR1" s="10"/>
+      <c r="MS1" s="10"/>
+      <c r="MT1" s="10"/>
+      <c r="MU1" s="10"/>
+      <c r="MV1" s="10"/>
+      <c r="MW1" s="10"/>
+      <c r="MX1" s="10"/>
+      <c r="MY1" s="10"/>
+      <c r="MZ1" s="10"/>
+      <c r="NA1" s="10"/>
+      <c r="NB1" s="10"/>
+      <c r="NC1" s="10"/>
+      <c r="ND1" s="10"/>
+      <c r="NE1" s="10"/>
+      <c r="NF1" s="10"/>
+      <c r="NG1" s="10"/>
+      <c r="NH1" s="10"/>
+      <c r="NI1" s="10"/>
+      <c r="NJ1" s="10"/>
+      <c r="NK1" s="10"/>
+      <c r="NL1" s="10"/>
+      <c r="NM1" s="10"/>
+      <c r="NN1" s="10"/>
+      <c r="NO1" s="10"/>
+      <c r="NP1" s="10"/>
+      <c r="NQ1" s="10"/>
+      <c r="NR1" s="10"/>
+      <c r="NS1" s="10"/>
+      <c r="NT1" s="10"/>
+      <c r="NU1" s="10"/>
+      <c r="NV1" s="10"/>
+      <c r="NW1" s="10"/>
+      <c r="NX1" s="10"/>
+      <c r="NY1" s="10"/>
+      <c r="NZ1" s="10"/>
+      <c r="OA1" s="10"/>
+      <c r="OB1" s="10"/>
+      <c r="OC1" s="10"/>
+      <c r="OD1" s="10"/>
+      <c r="OE1" s="10"/>
+      <c r="OF1" s="10"/>
+      <c r="OG1" s="10"/>
+      <c r="OH1" s="10"/>
+      <c r="OI1" s="10"/>
+      <c r="OJ1" s="10"/>
+      <c r="OK1" s="10"/>
+      <c r="OL1" s="10"/>
+      <c r="OM1" s="10"/>
+      <c r="ON1" s="10"/>
+      <c r="OO1" s="10"/>
+      <c r="OP1" s="10"/>
+      <c r="OQ1" s="10"/>
+      <c r="OR1" s="10"/>
+      <c r="OS1" s="10"/>
+      <c r="OT1" s="10"/>
+      <c r="OU1" s="10"/>
+      <c r="OV1" s="10"/>
+      <c r="OW1" s="10"/>
+      <c r="OX1" s="10"/>
+      <c r="OY1" s="10"/>
+      <c r="OZ1" s="10"/>
+      <c r="PA1" s="10"/>
+      <c r="PB1" s="10"/>
+      <c r="PC1" s="10"/>
+      <c r="PD1" s="10"/>
+      <c r="PE1" s="10"/>
+      <c r="PF1" s="10"/>
+      <c r="PG1" s="10"/>
+      <c r="PH1" s="10"/>
+      <c r="PI1" s="10"/>
+      <c r="PJ1" s="10"/>
+      <c r="PK1" s="10"/>
+      <c r="PL1" s="10"/>
+      <c r="PM1" s="10"/>
+      <c r="PN1" s="10"/>
+      <c r="PO1" s="10"/>
+      <c r="PP1" s="10"/>
+      <c r="PQ1" s="10"/>
+      <c r="PR1" s="10"/>
+      <c r="PS1" s="10"/>
+      <c r="PT1" s="10"/>
+      <c r="PU1" s="10"/>
+      <c r="PV1" s="10"/>
+      <c r="PW1" s="10"/>
+      <c r="PX1" s="10"/>
+      <c r="PY1" s="10"/>
+      <c r="PZ1" s="10"/>
+      <c r="QA1" s="10"/>
+      <c r="QB1" s="10"/>
+      <c r="QC1" s="10"/>
+      <c r="QD1" s="10"/>
+      <c r="QE1" s="10"/>
+      <c r="QF1" s="10"/>
+      <c r="QG1" s="10"/>
+      <c r="QH1" s="10"/>
+      <c r="QI1" s="10"/>
+      <c r="QJ1" s="10"/>
+      <c r="QK1" s="10"/>
+      <c r="QL1" s="10"/>
+      <c r="QM1" s="10"/>
+      <c r="QN1" s="10"/>
+      <c r="QO1" s="10"/>
+      <c r="QP1" s="10"/>
+      <c r="QQ1" s="10"/>
+      <c r="QR1" s="10"/>
+      <c r="QS1" s="10"/>
+      <c r="QT1" s="10"/>
+      <c r="QU1" s="10"/>
+      <c r="QV1" s="10"/>
+      <c r="QW1" s="10"/>
+      <c r="QX1" s="10"/>
+      <c r="QY1" s="10"/>
+      <c r="QZ1" s="10"/>
+      <c r="RA1" s="10"/>
+      <c r="RB1" s="10"/>
+      <c r="RC1" s="10"/>
+      <c r="RD1" s="10"/>
+      <c r="RE1" s="10"/>
+      <c r="RF1" s="10"/>
+      <c r="RG1" s="10"/>
+      <c r="RH1" s="10"/>
+      <c r="RI1" s="10"/>
+      <c r="RJ1" s="10"/>
+      <c r="RK1" s="10"/>
+      <c r="RL1" s="10"/>
+      <c r="RM1" s="10"/>
+      <c r="RN1" s="10"/>
+      <c r="RO1" s="10"/>
+      <c r="RP1" s="10"/>
+      <c r="RQ1" s="10"/>
+      <c r="RR1" s="10"/>
+      <c r="RS1" s="10"/>
+      <c r="RT1" s="10"/>
+      <c r="RU1" s="10"/>
+      <c r="RV1" s="10"/>
+      <c r="RW1" s="10"/>
+      <c r="RX1" s="10"/>
+      <c r="RY1" s="10"/>
+      <c r="RZ1" s="10"/>
+      <c r="SA1" s="10"/>
+      <c r="SB1" s="10"/>
+      <c r="SC1" s="10"/>
+      <c r="SD1" s="10"/>
+      <c r="SE1" s="10"/>
+      <c r="SF1" s="10"/>
+      <c r="SG1" s="10"/>
+      <c r="SH1" s="10"/>
+      <c r="SI1" s="10"/>
+      <c r="SJ1" s="10"/>
+      <c r="SK1" s="10"/>
+      <c r="SL1" s="10"/>
+      <c r="SM1" s="10"/>
+      <c r="SN1" s="10"/>
+      <c r="SO1" s="10"/>
+      <c r="SP1" s="10"/>
+      <c r="SQ1" s="10"/>
+      <c r="SR1" s="10"/>
+      <c r="SS1" s="10"/>
+      <c r="ST1" s="10"/>
+      <c r="SU1" s="10"/>
+      <c r="SV1" s="10"/>
+      <c r="SW1" s="10"/>
+      <c r="SX1" s="10"/>
+      <c r="SY1" s="10"/>
+      <c r="SZ1" s="10"/>
+      <c r="TA1" s="10"/>
+      <c r="TB1" s="10"/>
+      <c r="TC1" s="10"/>
+      <c r="TD1" s="10"/>
+      <c r="TE1" s="10"/>
+      <c r="TF1" s="10"/>
+      <c r="TG1" s="10"/>
+      <c r="TH1" s="10"/>
+      <c r="TI1" s="10"/>
+      <c r="TJ1" s="10"/>
+      <c r="TK1" s="10"/>
+      <c r="TL1" s="10"/>
+      <c r="TM1" s="10"/>
+      <c r="TN1" s="10"/>
+      <c r="TO1" s="10"/>
+      <c r="TP1" s="10"/>
+      <c r="TQ1" s="10"/>
+      <c r="TR1" s="10"/>
+      <c r="TS1" s="10"/>
+      <c r="TT1" s="10"/>
+      <c r="TU1" s="10"/>
+      <c r="TV1" s="10"/>
+      <c r="TW1" s="10"/>
+      <c r="TX1" s="10"/>
+      <c r="TY1" s="10"/>
+      <c r="TZ1" s="10"/>
+      <c r="UA1" s="10"/>
+      <c r="UB1" s="10"/>
+      <c r="UC1" s="10"/>
+      <c r="UD1" s="10"/>
+      <c r="UE1" s="10"/>
+      <c r="UF1" s="10"/>
+      <c r="UG1" s="10"/>
+      <c r="UH1" s="10"/>
+      <c r="UI1" s="10"/>
+      <c r="UJ1" s="10"/>
+      <c r="UK1" s="10"/>
+      <c r="UL1" s="10"/>
+      <c r="UM1" s="10"/>
+      <c r="UN1" s="10"/>
+      <c r="UO1" s="10"/>
+      <c r="UP1" s="10"/>
+      <c r="UQ1" s="10"/>
+      <c r="UR1" s="10"/>
+      <c r="US1" s="10"/>
+      <c r="UT1" s="10"/>
+      <c r="UU1" s="10"/>
+      <c r="UV1" s="10"/>
+      <c r="UW1" s="10"/>
+      <c r="UX1" s="10"/>
+      <c r="UY1" s="10"/>
+      <c r="UZ1" s="10"/>
+      <c r="VA1" s="10"/>
+      <c r="VB1" s="10"/>
+      <c r="VC1" s="10"/>
+      <c r="VD1" s="10"/>
+      <c r="VE1" s="10"/>
+      <c r="VF1" s="10"/>
+      <c r="VG1" s="10"/>
+      <c r="VH1" s="10"/>
+      <c r="VI1" s="10"/>
+      <c r="VJ1" s="10"/>
+      <c r="VK1" s="10"/>
+      <c r="VL1" s="10"/>
+      <c r="VM1" s="10"/>
+      <c r="VN1" s="10"/>
+      <c r="VO1" s="10"/>
+      <c r="VP1" s="10"/>
+      <c r="VQ1" s="10"/>
+      <c r="VR1" s="10"/>
+      <c r="VS1" s="10"/>
+      <c r="VT1" s="10"/>
+      <c r="VU1" s="10"/>
+      <c r="VV1" s="10"/>
+      <c r="VW1" s="10"/>
+      <c r="VX1" s="10"/>
+      <c r="VY1" s="10"/>
+      <c r="VZ1" s="10"/>
+      <c r="WA1" s="10"/>
+      <c r="WB1" s="10"/>
+      <c r="WC1" s="10"/>
+      <c r="WD1" s="10"/>
+      <c r="WE1" s="10"/>
+      <c r="WF1" s="10"/>
+      <c r="WG1" s="10"/>
+      <c r="WH1" s="10"/>
+      <c r="WI1" s="10"/>
+      <c r="WJ1" s="10"/>
+      <c r="WK1" s="10"/>
+      <c r="WL1" s="10"/>
+      <c r="WM1" s="10"/>
+      <c r="WN1" s="10"/>
+      <c r="WO1" s="10"/>
+      <c r="WP1" s="10"/>
+      <c r="WQ1" s="10"/>
+      <c r="WR1" s="10"/>
+      <c r="WS1" s="10"/>
+      <c r="WT1" s="10"/>
+      <c r="WU1" s="10"/>
+      <c r="WV1" s="10"/>
+      <c r="WW1" s="10"/>
+      <c r="WX1" s="10"/>
+      <c r="WY1" s="10"/>
+      <c r="WZ1" s="10"/>
+      <c r="XA1" s="10"/>
+      <c r="XB1" s="10"/>
+      <c r="XC1" s="10"/>
+      <c r="XD1" s="10"/>
+      <c r="XE1" s="10"/>
+      <c r="XF1" s="10"/>
+      <c r="XG1" s="10"/>
+      <c r="XH1" s="10"/>
+      <c r="XI1" s="10"/>
+      <c r="XJ1" s="10"/>
+      <c r="XK1" s="10"/>
+      <c r="XL1" s="10"/>
+      <c r="XM1" s="10"/>
+      <c r="XN1" s="10"/>
+      <c r="XO1" s="10"/>
+      <c r="XP1" s="10"/>
+      <c r="XQ1" s="10"/>
+      <c r="XR1" s="10"/>
+      <c r="XS1" s="10"/>
+      <c r="XT1" s="10"/>
+      <c r="XU1" s="10"/>
+      <c r="XV1" s="10"/>
+      <c r="XW1" s="10"/>
+      <c r="XX1" s="10"/>
+      <c r="XY1" s="10"/>
+      <c r="XZ1" s="10"/>
+      <c r="YA1" s="10"/>
+      <c r="YB1" s="10"/>
+      <c r="YC1" s="10"/>
+      <c r="YD1" s="10"/>
+      <c r="YE1" s="10"/>
+      <c r="YF1" s="10"/>
+      <c r="YG1" s="10"/>
+      <c r="YH1" s="10"/>
+      <c r="YI1" s="10"/>
+      <c r="YJ1" s="10"/>
+      <c r="YK1" s="10"/>
+      <c r="YL1" s="10"/>
+      <c r="YM1" s="10"/>
+      <c r="YN1" s="10"/>
+      <c r="YO1" s="10"/>
+      <c r="YP1" s="10"/>
+      <c r="YQ1" s="10"/>
+      <c r="YR1" s="10"/>
+      <c r="YS1" s="10"/>
+      <c r="YT1" s="10"/>
+      <c r="YU1" s="10"/>
+      <c r="YV1" s="10"/>
+      <c r="YW1" s="10"/>
+      <c r="YX1" s="10"/>
+      <c r="YY1" s="10"/>
+      <c r="YZ1" s="10"/>
+      <c r="ZA1" s="10"/>
+      <c r="ZB1" s="10"/>
+      <c r="ZC1" s="10"/>
+      <c r="ZD1" s="10"/>
+      <c r="ZE1" s="10"/>
+      <c r="ZF1" s="10"/>
+      <c r="ZG1" s="10"/>
+      <c r="ZH1" s="10"/>
+      <c r="ZI1" s="10"/>
+      <c r="ZJ1" s="10"/>
+      <c r="ZK1" s="10"/>
+      <c r="ZL1" s="10"/>
+      <c r="ZM1" s="10"/>
+      <c r="ZN1" s="10"/>
+      <c r="ZO1" s="10"/>
+      <c r="ZP1" s="10"/>
+      <c r="ZQ1" s="10"/>
+      <c r="ZR1" s="10"/>
+      <c r="ZS1" s="10"/>
+      <c r="ZT1" s="10"/>
+      <c r="ZU1" s="10"/>
+      <c r="ZV1" s="10"/>
+      <c r="ZW1" s="10"/>
+      <c r="ZX1" s="10"/>
+      <c r="ZY1" s="10"/>
+      <c r="ZZ1" s="10"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
@@ -5176,7 +5878,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3AF4C6E-3E65-4E26-AFB9-A800448A3220}">
-  <dimension ref="A1:N75"/>
+  <dimension ref="A1:ZZ75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -5191,48 +5893,736 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="11" t="s">
         <v>96</v>
       </c>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
+      <c r="AA1" s="11"/>
+      <c r="AB1" s="11"/>
+      <c r="AC1" s="11"/>
+      <c r="AD1" s="11"/>
+      <c r="AE1" s="11"/>
+      <c r="AF1" s="11"/>
+      <c r="AG1" s="11"/>
+      <c r="AH1" s="11"/>
+      <c r="AI1" s="11"/>
+      <c r="AJ1" s="11"/>
+      <c r="AK1" s="11"/>
+      <c r="AL1" s="11"/>
+      <c r="AM1" s="11"/>
+      <c r="AN1" s="11"/>
+      <c r="AO1" s="11"/>
+      <c r="AP1" s="11"/>
+      <c r="AQ1" s="11"/>
+      <c r="AR1" s="11"/>
+      <c r="AS1" s="11"/>
+      <c r="AT1" s="11"/>
+      <c r="AU1" s="11"/>
+      <c r="AV1" s="11"/>
+      <c r="AW1" s="11"/>
+      <c r="AX1" s="11"/>
+      <c r="AY1" s="11"/>
+      <c r="AZ1" s="11"/>
+      <c r="BA1" s="11"/>
+      <c r="BB1" s="11"/>
+      <c r="BC1" s="11"/>
+      <c r="BD1" s="11"/>
+      <c r="BE1" s="11"/>
+      <c r="BF1" s="11"/>
+      <c r="BG1" s="11"/>
+      <c r="BH1" s="11"/>
+      <c r="BI1" s="11"/>
+      <c r="BJ1" s="11"/>
+      <c r="BK1" s="11"/>
+      <c r="BL1" s="11"/>
+      <c r="BM1" s="11"/>
+      <c r="BN1" s="11"/>
+      <c r="BO1" s="11"/>
+      <c r="BP1" s="11"/>
+      <c r="BQ1" s="11"/>
+      <c r="BR1" s="11"/>
+      <c r="BS1" s="11"/>
+      <c r="BT1" s="11"/>
+      <c r="BU1" s="11"/>
+      <c r="BV1" s="11"/>
+      <c r="BW1" s="11"/>
+      <c r="BX1" s="11"/>
+      <c r="BY1" s="11"/>
+      <c r="BZ1" s="11"/>
+      <c r="CA1" s="11"/>
+      <c r="CB1" s="11"/>
+      <c r="CC1" s="11"/>
+      <c r="CD1" s="11"/>
+      <c r="CE1" s="11"/>
+      <c r="CF1" s="11"/>
+      <c r="CG1" s="11"/>
+      <c r="CH1" s="11"/>
+      <c r="CI1" s="11"/>
+      <c r="CJ1" s="11"/>
+      <c r="CK1" s="11"/>
+      <c r="CL1" s="11"/>
+      <c r="CM1" s="11"/>
+      <c r="CN1" s="11"/>
+      <c r="CO1" s="11"/>
+      <c r="CP1" s="11"/>
+      <c r="CQ1" s="11"/>
+      <c r="CR1" s="11"/>
+      <c r="CS1" s="11"/>
+      <c r="CT1" s="11"/>
+      <c r="CU1" s="11"/>
+      <c r="CV1" s="11"/>
+      <c r="CW1" s="11"/>
+      <c r="CX1" s="11"/>
+      <c r="CY1" s="11"/>
+      <c r="CZ1" s="11"/>
+      <c r="DA1" s="11"/>
+      <c r="DB1" s="11"/>
+      <c r="DC1" s="11"/>
+      <c r="DD1" s="11"/>
+      <c r="DE1" s="11"/>
+      <c r="DF1" s="11"/>
+      <c r="DG1" s="11"/>
+      <c r="DH1" s="11"/>
+      <c r="DI1" s="11"/>
+      <c r="DJ1" s="11"/>
+      <c r="DK1" s="11"/>
+      <c r="DL1" s="11"/>
+      <c r="DM1" s="11"/>
+      <c r="DN1" s="11"/>
+      <c r="DO1" s="11"/>
+      <c r="DP1" s="11"/>
+      <c r="DQ1" s="11"/>
+      <c r="DR1" s="11"/>
+      <c r="DS1" s="11"/>
+      <c r="DT1" s="11"/>
+      <c r="DU1" s="11"/>
+      <c r="DV1" s="11"/>
+      <c r="DW1" s="11"/>
+      <c r="DX1" s="11"/>
+      <c r="DY1" s="11"/>
+      <c r="DZ1" s="11"/>
+      <c r="EA1" s="11"/>
+      <c r="EB1" s="11"/>
+      <c r="EC1" s="11"/>
+      <c r="ED1" s="11"/>
+      <c r="EE1" s="11"/>
+      <c r="EF1" s="11"/>
+      <c r="EG1" s="11"/>
+      <c r="EH1" s="11"/>
+      <c r="EI1" s="11"/>
+      <c r="EJ1" s="11"/>
+      <c r="EK1" s="11"/>
+      <c r="EL1" s="11"/>
+      <c r="EM1" s="11"/>
+      <c r="EN1" s="11"/>
+      <c r="EO1" s="11"/>
+      <c r="EP1" s="11"/>
+      <c r="EQ1" s="11"/>
+      <c r="ER1" s="11"/>
+      <c r="ES1" s="11"/>
+      <c r="ET1" s="11"/>
+      <c r="EU1" s="11"/>
+      <c r="EV1" s="11"/>
+      <c r="EW1" s="11"/>
+      <c r="EX1" s="11"/>
+      <c r="EY1" s="11"/>
+      <c r="EZ1" s="11"/>
+      <c r="FA1" s="11"/>
+      <c r="FB1" s="11"/>
+      <c r="FC1" s="11"/>
+      <c r="FD1" s="11"/>
+      <c r="FE1" s="11"/>
+      <c r="FF1" s="11"/>
+      <c r="FG1" s="11"/>
+      <c r="FH1" s="11"/>
+      <c r="FI1" s="11"/>
+      <c r="FJ1" s="11"/>
+      <c r="FK1" s="11"/>
+      <c r="FL1" s="11"/>
+      <c r="FM1" s="11"/>
+      <c r="FN1" s="11"/>
+      <c r="FO1" s="11"/>
+      <c r="FP1" s="11"/>
+      <c r="FQ1" s="11"/>
+      <c r="FR1" s="11"/>
+      <c r="FS1" s="11"/>
+      <c r="FT1" s="11"/>
+      <c r="FU1" s="11"/>
+      <c r="FV1" s="11"/>
+      <c r="FW1" s="11"/>
+      <c r="FX1" s="11"/>
+      <c r="FY1" s="11"/>
+      <c r="FZ1" s="11"/>
+      <c r="GA1" s="11"/>
+      <c r="GB1" s="11"/>
+      <c r="GC1" s="11"/>
+      <c r="GD1" s="11"/>
+      <c r="GE1" s="11"/>
+      <c r="GF1" s="11"/>
+      <c r="GG1" s="11"/>
+      <c r="GH1" s="11"/>
+      <c r="GI1" s="11"/>
+      <c r="GJ1" s="11"/>
+      <c r="GK1" s="11"/>
+      <c r="GL1" s="11"/>
+      <c r="GM1" s="11"/>
+      <c r="GN1" s="11"/>
+      <c r="GO1" s="11"/>
+      <c r="GP1" s="11"/>
+      <c r="GQ1" s="11"/>
+      <c r="GR1" s="11"/>
+      <c r="GS1" s="11"/>
+      <c r="GT1" s="11"/>
+      <c r="GU1" s="11"/>
+      <c r="GV1" s="11"/>
+      <c r="GW1" s="11"/>
+      <c r="GX1" s="11"/>
+      <c r="GY1" s="11"/>
+      <c r="GZ1" s="11"/>
+      <c r="HA1" s="11"/>
+      <c r="HB1" s="11"/>
+      <c r="HC1" s="11"/>
+      <c r="HD1" s="11"/>
+      <c r="HE1" s="11"/>
+      <c r="HF1" s="11"/>
+      <c r="HG1" s="11"/>
+      <c r="HH1" s="11"/>
+      <c r="HI1" s="11"/>
+      <c r="HJ1" s="11"/>
+      <c r="HK1" s="11"/>
+      <c r="HL1" s="11"/>
+      <c r="HM1" s="11"/>
+      <c r="HN1" s="11"/>
+      <c r="HO1" s="11"/>
+      <c r="HP1" s="11"/>
+      <c r="HQ1" s="11"/>
+      <c r="HR1" s="11"/>
+      <c r="HS1" s="11"/>
+      <c r="HT1" s="11"/>
+      <c r="HU1" s="11"/>
+      <c r="HV1" s="11"/>
+      <c r="HW1" s="11"/>
+      <c r="HX1" s="11"/>
+      <c r="HY1" s="11"/>
+      <c r="HZ1" s="11"/>
+      <c r="IA1" s="11"/>
+      <c r="IB1" s="11"/>
+      <c r="IC1" s="11"/>
+      <c r="ID1" s="11"/>
+      <c r="IE1" s="11"/>
+      <c r="IF1" s="11"/>
+      <c r="IG1" s="11"/>
+      <c r="IH1" s="11"/>
+      <c r="II1" s="11"/>
+      <c r="IJ1" s="11"/>
+      <c r="IK1" s="11"/>
+      <c r="IL1" s="11"/>
+      <c r="IM1" s="11"/>
+      <c r="IN1" s="11"/>
+      <c r="IO1" s="11"/>
+      <c r="IP1" s="11"/>
+      <c r="IQ1" s="11"/>
+      <c r="IR1" s="11"/>
+      <c r="IS1" s="11"/>
+      <c r="IT1" s="11"/>
+      <c r="IU1" s="11"/>
+      <c r="IV1" s="11"/>
+      <c r="IW1" s="11"/>
+      <c r="IX1" s="11"/>
+      <c r="IY1" s="11"/>
+      <c r="IZ1" s="11"/>
+      <c r="JA1" s="11"/>
+      <c r="JB1" s="11"/>
+      <c r="JC1" s="11"/>
+      <c r="JD1" s="11"/>
+      <c r="JE1" s="11"/>
+      <c r="JF1" s="11"/>
+      <c r="JG1" s="11"/>
+      <c r="JH1" s="11"/>
+      <c r="JI1" s="11"/>
+      <c r="JJ1" s="11"/>
+      <c r="JK1" s="11"/>
+      <c r="JL1" s="11"/>
+      <c r="JM1" s="11"/>
+      <c r="JN1" s="11"/>
+      <c r="JO1" s="11"/>
+      <c r="JP1" s="11"/>
+      <c r="JQ1" s="11"/>
+      <c r="JR1" s="11"/>
+      <c r="JS1" s="11"/>
+      <c r="JT1" s="11"/>
+      <c r="JU1" s="11"/>
+      <c r="JV1" s="11"/>
+      <c r="JW1" s="11"/>
+      <c r="JX1" s="11"/>
+      <c r="JY1" s="11"/>
+      <c r="JZ1" s="11"/>
+      <c r="KA1" s="11"/>
+      <c r="KB1" s="11"/>
+      <c r="KC1" s="11"/>
+      <c r="KD1" s="11"/>
+      <c r="KE1" s="11"/>
+      <c r="KF1" s="11"/>
+      <c r="KG1" s="11"/>
+      <c r="KH1" s="11"/>
+      <c r="KI1" s="11"/>
+      <c r="KJ1" s="11"/>
+      <c r="KK1" s="11"/>
+      <c r="KL1" s="11"/>
+      <c r="KM1" s="11"/>
+      <c r="KN1" s="11"/>
+      <c r="KO1" s="11"/>
+      <c r="KP1" s="11"/>
+      <c r="KQ1" s="11"/>
+      <c r="KR1" s="11"/>
+      <c r="KS1" s="11"/>
+      <c r="KT1" s="11"/>
+      <c r="KU1" s="11"/>
+      <c r="KV1" s="11"/>
+      <c r="KW1" s="11"/>
+      <c r="KX1" s="11"/>
+      <c r="KY1" s="11"/>
+      <c r="KZ1" s="11"/>
+      <c r="LA1" s="11"/>
+      <c r="LB1" s="11"/>
+      <c r="LC1" s="11"/>
+      <c r="LD1" s="11"/>
+      <c r="LE1" s="11"/>
+      <c r="LF1" s="11"/>
+      <c r="LG1" s="11"/>
+      <c r="LH1" s="11"/>
+      <c r="LI1" s="11"/>
+      <c r="LJ1" s="11"/>
+      <c r="LK1" s="11"/>
+      <c r="LL1" s="11"/>
+      <c r="LM1" s="11"/>
+      <c r="LN1" s="11"/>
+      <c r="LO1" s="11"/>
+      <c r="LP1" s="11"/>
+      <c r="LQ1" s="11"/>
+      <c r="LR1" s="11"/>
+      <c r="LS1" s="11"/>
+      <c r="LT1" s="11"/>
+      <c r="LU1" s="11"/>
+      <c r="LV1" s="11"/>
+      <c r="LW1" s="11"/>
+      <c r="LX1" s="11"/>
+      <c r="LY1" s="11"/>
+      <c r="LZ1" s="11"/>
+      <c r="MA1" s="11"/>
+      <c r="MB1" s="11"/>
+      <c r="MC1" s="11"/>
+      <c r="MD1" s="11"/>
+      <c r="ME1" s="11"/>
+      <c r="MF1" s="11"/>
+      <c r="MG1" s="11"/>
+      <c r="MH1" s="11"/>
+      <c r="MI1" s="11"/>
+      <c r="MJ1" s="11"/>
+      <c r="MK1" s="11"/>
+      <c r="ML1" s="11"/>
+      <c r="MM1" s="11"/>
+      <c r="MN1" s="11"/>
+      <c r="MO1" s="11"/>
+      <c r="MP1" s="11"/>
+      <c r="MQ1" s="11"/>
+      <c r="MR1" s="11"/>
+      <c r="MS1" s="11"/>
+      <c r="MT1" s="11"/>
+      <c r="MU1" s="11"/>
+      <c r="MV1" s="11"/>
+      <c r="MW1" s="11"/>
+      <c r="MX1" s="11"/>
+      <c r="MY1" s="11"/>
+      <c r="MZ1" s="11"/>
+      <c r="NA1" s="11"/>
+      <c r="NB1" s="11"/>
+      <c r="NC1" s="11"/>
+      <c r="ND1" s="11"/>
+      <c r="NE1" s="11"/>
+      <c r="NF1" s="11"/>
+      <c r="NG1" s="11"/>
+      <c r="NH1" s="11"/>
+      <c r="NI1" s="11"/>
+      <c r="NJ1" s="11"/>
+      <c r="NK1" s="11"/>
+      <c r="NL1" s="11"/>
+      <c r="NM1" s="11"/>
+      <c r="NN1" s="11"/>
+      <c r="NO1" s="11"/>
+      <c r="NP1" s="11"/>
+      <c r="NQ1" s="11"/>
+      <c r="NR1" s="11"/>
+      <c r="NS1" s="11"/>
+      <c r="NT1" s="11"/>
+      <c r="NU1" s="11"/>
+      <c r="NV1" s="11"/>
+      <c r="NW1" s="11"/>
+      <c r="NX1" s="11"/>
+      <c r="NY1" s="11"/>
+      <c r="NZ1" s="11"/>
+      <c r="OA1" s="11"/>
+      <c r="OB1" s="11"/>
+      <c r="OC1" s="11"/>
+      <c r="OD1" s="11"/>
+      <c r="OE1" s="11"/>
+      <c r="OF1" s="11"/>
+      <c r="OG1" s="11"/>
+      <c r="OH1" s="11"/>
+      <c r="OI1" s="11"/>
+      <c r="OJ1" s="11"/>
+      <c r="OK1" s="11"/>
+      <c r="OL1" s="11"/>
+      <c r="OM1" s="11"/>
+      <c r="ON1" s="11"/>
+      <c r="OO1" s="11"/>
+      <c r="OP1" s="11"/>
+      <c r="OQ1" s="11"/>
+      <c r="OR1" s="11"/>
+      <c r="OS1" s="11"/>
+      <c r="OT1" s="11"/>
+      <c r="OU1" s="11"/>
+      <c r="OV1" s="11"/>
+      <c r="OW1" s="11"/>
+      <c r="OX1" s="11"/>
+      <c r="OY1" s="11"/>
+      <c r="OZ1" s="11"/>
+      <c r="PA1" s="11"/>
+      <c r="PB1" s="11"/>
+      <c r="PC1" s="11"/>
+      <c r="PD1" s="11"/>
+      <c r="PE1" s="11"/>
+      <c r="PF1" s="11"/>
+      <c r="PG1" s="11"/>
+      <c r="PH1" s="11"/>
+      <c r="PI1" s="11"/>
+      <c r="PJ1" s="11"/>
+      <c r="PK1" s="11"/>
+      <c r="PL1" s="11"/>
+      <c r="PM1" s="11"/>
+      <c r="PN1" s="11"/>
+      <c r="PO1" s="11"/>
+      <c r="PP1" s="11"/>
+      <c r="PQ1" s="11"/>
+      <c r="PR1" s="11"/>
+      <c r="PS1" s="11"/>
+      <c r="PT1" s="11"/>
+      <c r="PU1" s="11"/>
+      <c r="PV1" s="11"/>
+      <c r="PW1" s="11"/>
+      <c r="PX1" s="11"/>
+      <c r="PY1" s="11"/>
+      <c r="PZ1" s="11"/>
+      <c r="QA1" s="11"/>
+      <c r="QB1" s="11"/>
+      <c r="QC1" s="11"/>
+      <c r="QD1" s="11"/>
+      <c r="QE1" s="11"/>
+      <c r="QF1" s="11"/>
+      <c r="QG1" s="11"/>
+      <c r="QH1" s="11"/>
+      <c r="QI1" s="11"/>
+      <c r="QJ1" s="11"/>
+      <c r="QK1" s="11"/>
+      <c r="QL1" s="11"/>
+      <c r="QM1" s="11"/>
+      <c r="QN1" s="11"/>
+      <c r="QO1" s="11"/>
+      <c r="QP1" s="11"/>
+      <c r="QQ1" s="11"/>
+      <c r="QR1" s="11"/>
+      <c r="QS1" s="11"/>
+      <c r="QT1" s="11"/>
+      <c r="QU1" s="11"/>
+      <c r="QV1" s="11"/>
+      <c r="QW1" s="11"/>
+      <c r="QX1" s="11"/>
+      <c r="QY1" s="11"/>
+      <c r="QZ1" s="11"/>
+      <c r="RA1" s="11"/>
+      <c r="RB1" s="11"/>
+      <c r="RC1" s="11"/>
+      <c r="RD1" s="11"/>
+      <c r="RE1" s="11"/>
+      <c r="RF1" s="11"/>
+      <c r="RG1" s="11"/>
+      <c r="RH1" s="11"/>
+      <c r="RI1" s="11"/>
+      <c r="RJ1" s="11"/>
+      <c r="RK1" s="11"/>
+      <c r="RL1" s="11"/>
+      <c r="RM1" s="11"/>
+      <c r="RN1" s="11"/>
+      <c r="RO1" s="11"/>
+      <c r="RP1" s="11"/>
+      <c r="RQ1" s="11"/>
+      <c r="RR1" s="11"/>
+      <c r="RS1" s="11"/>
+      <c r="RT1" s="11"/>
+      <c r="RU1" s="11"/>
+      <c r="RV1" s="11"/>
+      <c r="RW1" s="11"/>
+      <c r="RX1" s="11"/>
+      <c r="RY1" s="11"/>
+      <c r="RZ1" s="11"/>
+      <c r="SA1" s="11"/>
+      <c r="SB1" s="11"/>
+      <c r="SC1" s="11"/>
+      <c r="SD1" s="11"/>
+      <c r="SE1" s="11"/>
+      <c r="SF1" s="11"/>
+      <c r="SG1" s="11"/>
+      <c r="SH1" s="11"/>
+      <c r="SI1" s="11"/>
+      <c r="SJ1" s="11"/>
+      <c r="SK1" s="11"/>
+      <c r="SL1" s="11"/>
+      <c r="SM1" s="11"/>
+      <c r="SN1" s="11"/>
+      <c r="SO1" s="11"/>
+      <c r="SP1" s="11"/>
+      <c r="SQ1" s="11"/>
+      <c r="SR1" s="11"/>
+      <c r="SS1" s="11"/>
+      <c r="ST1" s="11"/>
+      <c r="SU1" s="11"/>
+      <c r="SV1" s="11"/>
+      <c r="SW1" s="11"/>
+      <c r="SX1" s="11"/>
+      <c r="SY1" s="11"/>
+      <c r="SZ1" s="11"/>
+      <c r="TA1" s="11"/>
+      <c r="TB1" s="11"/>
+      <c r="TC1" s="11"/>
+      <c r="TD1" s="11"/>
+      <c r="TE1" s="11"/>
+      <c r="TF1" s="11"/>
+      <c r="TG1" s="11"/>
+      <c r="TH1" s="11"/>
+      <c r="TI1" s="11"/>
+      <c r="TJ1" s="11"/>
+      <c r="TK1" s="11"/>
+      <c r="TL1" s="11"/>
+      <c r="TM1" s="11"/>
+      <c r="TN1" s="11"/>
+      <c r="TO1" s="11"/>
+      <c r="TP1" s="11"/>
+      <c r="TQ1" s="11"/>
+      <c r="TR1" s="11"/>
+      <c r="TS1" s="11"/>
+      <c r="TT1" s="11"/>
+      <c r="TU1" s="11"/>
+      <c r="TV1" s="11"/>
+      <c r="TW1" s="11"/>
+      <c r="TX1" s="11"/>
+      <c r="TY1" s="11"/>
+      <c r="TZ1" s="11"/>
+      <c r="UA1" s="11"/>
+      <c r="UB1" s="11"/>
+      <c r="UC1" s="11"/>
+      <c r="UD1" s="11"/>
+      <c r="UE1" s="11"/>
+      <c r="UF1" s="11"/>
+      <c r="UG1" s="11"/>
+      <c r="UH1" s="11"/>
+      <c r="UI1" s="11"/>
+      <c r="UJ1" s="11"/>
+      <c r="UK1" s="11"/>
+      <c r="UL1" s="11"/>
+      <c r="UM1" s="11"/>
+      <c r="UN1" s="11"/>
+      <c r="UO1" s="11"/>
+      <c r="UP1" s="11"/>
+      <c r="UQ1" s="11"/>
+      <c r="UR1" s="11"/>
+      <c r="US1" s="11"/>
+      <c r="UT1" s="11"/>
+      <c r="UU1" s="11"/>
+      <c r="UV1" s="11"/>
+      <c r="UW1" s="11"/>
+      <c r="UX1" s="11"/>
+      <c r="UY1" s="11"/>
+      <c r="UZ1" s="11"/>
+      <c r="VA1" s="11"/>
+      <c r="VB1" s="11"/>
+      <c r="VC1" s="11"/>
+      <c r="VD1" s="11"/>
+      <c r="VE1" s="11"/>
+      <c r="VF1" s="11"/>
+      <c r="VG1" s="11"/>
+      <c r="VH1" s="11"/>
+      <c r="VI1" s="11"/>
+      <c r="VJ1" s="11"/>
+      <c r="VK1" s="11"/>
+      <c r="VL1" s="11"/>
+      <c r="VM1" s="11"/>
+      <c r="VN1" s="11"/>
+      <c r="VO1" s="11"/>
+      <c r="VP1" s="11"/>
+      <c r="VQ1" s="11"/>
+      <c r="VR1" s="11"/>
+      <c r="VS1" s="11"/>
+      <c r="VT1" s="11"/>
+      <c r="VU1" s="11"/>
+      <c r="VV1" s="11"/>
+      <c r="VW1" s="11"/>
+      <c r="VX1" s="11"/>
+      <c r="VY1" s="11"/>
+      <c r="VZ1" s="11"/>
+      <c r="WA1" s="11"/>
+      <c r="WB1" s="11"/>
+      <c r="WC1" s="11"/>
+      <c r="WD1" s="11"/>
+      <c r="WE1" s="11"/>
+      <c r="WF1" s="11"/>
+      <c r="WG1" s="11"/>
+      <c r="WH1" s="11"/>
+      <c r="WI1" s="11"/>
+      <c r="WJ1" s="11"/>
+      <c r="WK1" s="11"/>
+      <c r="WL1" s="11"/>
+      <c r="WM1" s="11"/>
+      <c r="WN1" s="11"/>
+      <c r="WO1" s="11"/>
+      <c r="WP1" s="11"/>
+      <c r="WQ1" s="11"/>
+      <c r="WR1" s="11"/>
+      <c r="WS1" s="11"/>
+      <c r="WT1" s="11"/>
+      <c r="WU1" s="11"/>
+      <c r="WV1" s="11"/>
+      <c r="WW1" s="11"/>
+      <c r="WX1" s="11"/>
+      <c r="WY1" s="11"/>
+      <c r="WZ1" s="11"/>
+      <c r="XA1" s="11"/>
+      <c r="XB1" s="11"/>
+      <c r="XC1" s="11"/>
+      <c r="XD1" s="11"/>
+      <c r="XE1" s="11"/>
+      <c r="XF1" s="11"/>
+      <c r="XG1" s="11"/>
+      <c r="XH1" s="11"/>
+      <c r="XI1" s="11"/>
+      <c r="XJ1" s="11"/>
+      <c r="XK1" s="11"/>
+      <c r="XL1" s="11"/>
+      <c r="XM1" s="11"/>
+      <c r="XN1" s="11"/>
+      <c r="XO1" s="11"/>
+      <c r="XP1" s="11"/>
+      <c r="XQ1" s="11"/>
+      <c r="XR1" s="11"/>
+      <c r="XS1" s="11"/>
+      <c r="XT1" s="11"/>
+      <c r="XU1" s="11"/>
+      <c r="XV1" s="11"/>
+      <c r="XW1" s="11"/>
+      <c r="XX1" s="11"/>
+      <c r="XY1" s="11"/>
+      <c r="XZ1" s="11"/>
+      <c r="YA1" s="11"/>
+      <c r="YB1" s="11"/>
+      <c r="YC1" s="11"/>
+      <c r="YD1" s="11"/>
+      <c r="YE1" s="11"/>
+      <c r="YF1" s="11"/>
+      <c r="YG1" s="11"/>
+      <c r="YH1" s="11"/>
+      <c r="YI1" s="11"/>
+      <c r="YJ1" s="11"/>
+      <c r="YK1" s="11"/>
+      <c r="YL1" s="11"/>
+      <c r="YM1" s="11"/>
+      <c r="YN1" s="11"/>
+      <c r="YO1" s="11"/>
+      <c r="YP1" s="11"/>
+      <c r="YQ1" s="11"/>
+      <c r="YR1" s="11"/>
+      <c r="YS1" s="11"/>
+      <c r="YT1" s="11"/>
+      <c r="YU1" s="11"/>
+      <c r="YV1" s="11"/>
+      <c r="YW1" s="11"/>
+      <c r="YX1" s="11"/>
+      <c r="YY1" s="11"/>
+      <c r="YZ1" s="11"/>
+      <c r="ZA1" s="11"/>
+      <c r="ZB1" s="11"/>
+      <c r="ZC1" s="11"/>
+      <c r="ZD1" s="11"/>
+      <c r="ZE1" s="11"/>
+      <c r="ZF1" s="11"/>
+      <c r="ZG1" s="11"/>
+      <c r="ZH1" s="11"/>
+      <c r="ZI1" s="11"/>
+      <c r="ZJ1" s="11"/>
+      <c r="ZK1" s="11"/>
+      <c r="ZL1" s="11"/>
+      <c r="ZM1" s="11"/>
+      <c r="ZN1" s="11"/>
+      <c r="ZO1" s="11"/>
+      <c r="ZP1" s="11"/>
+      <c r="ZQ1" s="11"/>
+      <c r="ZR1" s="11"/>
+      <c r="ZS1" s="11"/>
+      <c r="ZT1" s="11"/>
+      <c r="ZU1" s="11"/>
+      <c r="ZV1" s="11"/>
+      <c r="ZW1" s="11"/>
+      <c r="ZX1" s="11"/>
+      <c r="ZY1" s="11"/>
+      <c r="ZZ1" s="11"/>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">

</xml_diff>